<commit_message>
Fix error in BIM data (from Gigi)
</commit_message>
<xml_diff>
--- a/data/tle/2020-03-09_BIM.xlsx
+++ b/data/tle/2020-03-09_BIM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFB61E-1CC9-DF48-96C8-D5D2ED52F5A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A8D141-0A52-3A4E-BD29-B7E24C734E61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15960" xr2:uid="{FD8B587E-877F-9942-86B6-E4FDE0D90787}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Frag.</t>
   </si>
@@ -281,17 +281,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,7 +610,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,20 +633,20 @@
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
       <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
@@ -654,20 +654,20 @@
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>43899</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="9"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
       <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="11">
         <v>43899</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
@@ -675,20 +675,20 @@
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="10"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
@@ -706,10 +706,10 @@
       <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>148</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
@@ -752,7 +752,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="13">
         <v>133</v>
       </c>
       <c r="B6" s="3">
@@ -761,7 +761,7 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="13">
         <v>134</v>
       </c>
       <c r="E6" s="3">
@@ -770,7 +770,7 @@
       <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="13">
         <v>51</v>
       </c>
       <c r="H6" s="3">
@@ -779,7 +779,7 @@
       <c r="I6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="13">
         <v>52</v>
       </c>
       <c r="K6" s="3">
@@ -790,28 +790,28 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="3">
         <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="3">
         <v>2</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="3">
         <v>2</v>
       </c>
@@ -820,28 +820,28 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3">
         <v>3</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="3">
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="3">
         <v>3</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="3">
         <v>3</v>
       </c>
@@ -850,28 +850,28 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3">
         <v>4</v>
       </c>
       <c r="C9" s="3">
         <v>3</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="3">
         <v>4</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="3">
         <v>4</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="3">
         <v>4</v>
       </c>
@@ -880,28 +880,28 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3">
         <v>5</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="3">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="3">
         <v>5</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="3">
         <v>5</v>
       </c>
@@ -910,7 +910,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="13">
         <v>125</v>
       </c>
       <c r="B11" s="3">
@@ -919,7 +919,7 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="3">
@@ -928,7 +928,7 @@
       <c r="F11" s="3">
         <v>6</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="13">
         <v>53</v>
       </c>
       <c r="H11" s="3">
@@ -937,7 +937,7 @@
       <c r="I11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="13">
         <v>54</v>
       </c>
       <c r="K11" s="3">
@@ -948,28 +948,28 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="3">
         <v>2</v>
       </c>
       <c r="F12" s="3">
         <v>4</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="3">
         <v>2</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="3">
         <v>2</v>
       </c>
@@ -978,28 +978,28 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13" s="3">
         <v>4</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="3">
         <v>3</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="3">
         <v>3</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="3">
         <v>3</v>
       </c>
@@ -1008,28 +1008,28 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="3">
         <v>4</v>
       </c>
       <c r="C14" s="3">
         <v>4</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="3">
         <v>4</v>
       </c>
       <c r="F14" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="3">
         <v>4</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="10"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="3">
         <v>4</v>
       </c>
@@ -1038,28 +1038,28 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="3">
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="3">
         <v>5</v>
       </c>
       <c r="F15" s="3">
         <v>4</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="3">
         <v>5</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="10"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="3">
         <v>5</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="13">
         <v>94</v>
       </c>
       <c r="B16" s="3">
@@ -1077,7 +1077,7 @@
       <c r="C16" s="3">
         <v>4</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="13">
         <v>95</v>
       </c>
       <c r="E16" s="3">
@@ -1086,7 +1086,7 @@
       <c r="F16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="13">
         <v>55</v>
       </c>
       <c r="H16" s="3">
@@ -1095,7 +1095,7 @@
       <c r="I16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="13">
         <v>43</v>
       </c>
       <c r="K16" s="3">
@@ -1106,28 +1106,28 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="3">
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="3">
         <v>2</v>
       </c>
       <c r="F17" s="3">
         <v>9</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="3">
         <v>2</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="10"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="3">
         <v>2</v>
       </c>
@@ -1136,28 +1136,28 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="3">
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="3">
         <v>3</v>
       </c>
       <c r="F18" s="3">
         <v>16</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="3">
         <v>3</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="10"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="3">
         <v>3</v>
       </c>
@@ -1166,67 +1166,67 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="3">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="3">
         <v>4</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="3">
         <v>4</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="3">
         <v>4</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>18</v>
+      <c r="L19" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="3">
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="3">
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="3">
         <v>5</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="10"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="3">
         <v>5</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
+      <c r="A21" s="13">
         <v>96</v>
       </c>
       <c r="B21" s="3">
@@ -1235,7 +1235,7 @@
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="3">
@@ -1244,7 +1244,7 @@
       <c r="F21" s="3">
         <v>6</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="13">
         <v>49</v>
       </c>
       <c r="H21" s="3">
@@ -1253,7 +1253,7 @@
       <c r="I21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="13">
         <v>42</v>
       </c>
       <c r="K21" s="3">
@@ -1264,28 +1264,28 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="3">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="3">
         <v>2</v>
       </c>
       <c r="F22" s="3">
         <v>5</v>
       </c>
-      <c r="G22" s="10"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="3">
         <v>2</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="10"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="3">
         <v>2</v>
       </c>
@@ -1294,28 +1294,28 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="3">
         <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="3">
         <v>3</v>
       </c>
       <c r="F23" s="3">
         <v>6</v>
       </c>
-      <c r="G23" s="10"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="3">
         <v>3</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="10"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="3">
         <v>3</v>
       </c>
@@ -1324,28 +1324,28 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="3">
         <v>4</v>
       </c>
       <c r="C24" s="3">
         <v>14</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="3">
         <v>4</v>
       </c>
       <c r="F24" s="3">
         <v>4</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="3">
         <v>4</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="10"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="3">
         <v>4</v>
       </c>
@@ -1354,28 +1354,28 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="3">
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="3">
         <v>5</v>
       </c>
       <c r="F25" s="3">
         <v>8</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="3">
         <v>5</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="10"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="3">
         <v>5</v>
       </c>
@@ -1384,7 +1384,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="3">
@@ -1393,14 +1393,14 @@
       <c r="C26" s="3">
         <v>7</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="10">
+      <c r="G26" s="13">
         <v>44</v>
       </c>
       <c r="H26" s="3">
@@ -1409,7 +1409,7 @@
       <c r="I26" s="3">
         <v>3</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="13">
         <v>45</v>
       </c>
       <c r="K26" s="3">
@@ -1420,26 +1420,26 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="3">
         <v>2</v>
       </c>
       <c r="C27" s="3">
         <v>7</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="3">
         <v>2</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="10"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="3">
         <v>2</v>
       </c>
       <c r="I27" s="3">
         <v>5</v>
       </c>
-      <c r="J27" s="10"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="3">
         <v>2</v>
       </c>
@@ -1448,26 +1448,26 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="3">
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="3">
         <v>3</v>
       </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="10"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="3">
         <v>3</v>
       </c>
       <c r="I28" s="3">
         <v>5</v>
       </c>
-      <c r="J28" s="10"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="3">
         <v>3</v>
       </c>
@@ -1476,26 +1476,26 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="3">
         <v>4</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="3">
         <v>4</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="3">
         <v>4</v>
       </c>
       <c r="I29" s="3">
         <v>3</v>
       </c>
-      <c r="J29" s="10"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="3">
         <v>4</v>
       </c>
@@ -1504,26 +1504,26 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="3">
         <v>5</v>
       </c>
       <c r="C30" s="3">
         <v>4</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="3">
         <v>5</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="10"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="3">
         <v>5</v>
       </c>
       <c r="I30" s="3">
         <v>4</v>
       </c>
-      <c r="J30" s="10"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="3">
         <v>5</v>
       </c>
@@ -1733,6 +1733,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A26:A30"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1741,26 +1761,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="G21:G25"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="J16:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>